<commit_message>
cria modelo em pedidos e sobe arquivos excel
</commit_message>
<xml_diff>
--- a/app/Private/excel/itinerarios_admin.xlsx
+++ b/app/Private/excel/itinerarios_admin.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="61">
   <si>
     <t>CNPJ</t>
   </si>
@@ -195,6 +195,9 @@
   </si>
   <si>
     <t>Data</t>
+  </si>
+  <si>
+    <t>Codigo Operadora</t>
   </si>
 </sst>
 </file>
@@ -533,7 +536,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:BH1"/>
+  <dimension ref="A1:BI1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -541,7 +544,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" spans="1:60">
+    <row r="1" spans="1:61">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -721,6 +724,9 @@
       </c>
       <c r="BH1" t="s">
         <v>59</v>
+      </c>
+      <c r="BI1" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ajusta filtro relatorio periodos
</commit_message>
<xml_diff>
--- a/app/Private/excel/itinerarios_admin.xlsx
+++ b/app/Private/excel/itinerarios_admin.xlsx
@@ -221,10 +221,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
@@ -235,7 +232,7 @@
   </cellStyleXfs>
   <cellXfs count="1">
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+      <alignment vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -742,5 +739,6 @@
     <firstHeader/>
     <firstFooter/>
   </headerFooter>
+  <tableParts count="0"/>
 </worksheet>
 </file>
</xml_diff>